<commit_message>
compensate for barrel weight increase by reducing weight of some parts
</commit_message>
<xml_diff>
--- a/changes/9mm-mags.xlsx
+++ b/changes/9mm-mags.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94B1EEA-4B12-4985-B176-EA39B5C663F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7E2931-F945-46C6-9009-33C1096E448B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="556-mags" sheetId="1" r:id="rId1"/>
+    <sheet name="9mm-mags" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
   <si>
     <t>new</t>
   </si>
@@ -89,24 +89,12 @@
     <t>formula</t>
   </si>
   <si>
-    <t>glock17_9x19_stick_31r_magazine</t>
-  </si>
-  <si>
     <t>Glock 9x19 31R Stick</t>
   </si>
   <si>
     <t>9x19_glock_stick_31r</t>
   </si>
   <si>
-    <t>glock17_gen5_9x19_17r_magazine</t>
-  </si>
-  <si>
-    <t>Glock 9x19 17R</t>
-  </si>
-  <si>
-    <t>sgm_tactical_glock_9x19_50r_drum_magazine</t>
-  </si>
-  <si>
     <t>SGMT 9x19 50R Drum</t>
   </si>
   <si>
@@ -285,6 +273,24 @@
   </si>
   <si>
     <t>Glock 17R Magazine Bottom Plate</t>
+  </si>
+  <si>
+    <t>pf940_9x19_stick_31r_magazine</t>
+  </si>
+  <si>
+    <t>pf940_gen5_9x19_17r_magazine</t>
+  </si>
+  <si>
+    <t>sgm_tactical_pf940_9x19_50r_drum_magazine</t>
+  </si>
+  <si>
+    <t>9x19_kriss_magex2_vector</t>
+  </si>
+  <si>
+    <t>PF940 9x19 31R Stick</t>
+  </si>
+  <si>
+    <t>PF940 9x19 17R</t>
   </si>
 </sst>
 </file>
@@ -562,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T997"/>
+  <dimension ref="A1:T998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -655,10 +661,10 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="C3" s="2">
         <v>-3</v>
@@ -680,7 +686,7 @@
         <v>1000</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N73" si="0">C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300+G3/1.3</f>
+        <f t="shared" ref="N3:N74" si="0">C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300+G3/1.3</f>
         <v>13.846153846153847</v>
       </c>
       <c r="O3" s="1"/>
@@ -689,7 +695,7 @@
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1">
-        <f t="shared" ref="R3:R35" si="1">P3*0.024</f>
+        <f t="shared" ref="R3:R36" si="1">P3*0.024</f>
         <v>0.45600000000000002</v>
       </c>
       <c r="S3" s="1"/>
@@ -697,10 +703,10 @@
     </row>
     <row r="4" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2">
         <v>-3</v>
@@ -737,10 +743,10 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -779,10 +785,10 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2">
         <v>-7</v>
@@ -821,10 +827,10 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
         <v>-7</v>
@@ -861,10 +867,10 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -891,16 +897,16 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C9">
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="D9">
-        <v>0.27</v>
+        <v>0.3</v>
       </c>
       <c r="G9">
         <v>23</v>
@@ -910,7 +916,7 @@
       </c>
       <c r="N9" s="1">
         <f t="shared" si="0"/>
-        <v>6.292307692307693</v>
+        <v>3.6923076923076934</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -923,22 +929,27 @@
       <c r="T9" s="1"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10">
+        <v>-8</v>
+      </c>
+      <c r="D10">
+        <v>0.3</v>
+      </c>
+      <c r="G10">
+        <v>23</v>
+      </c>
+      <c r="M10">
+        <v>1000</v>
+      </c>
       <c r="N10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.6923076923076934</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -951,64 +962,34 @@
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0.02</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.4</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="2">
-        <v>-5</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.21</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2">
-        <v>18</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2">
-        <v>1000</v>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0.02</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
       </c>
       <c r="N12" s="1">
         <f t="shared" si="0"/>
-        <v>4.6461538461538456</v>
+        <v>-0.4</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -1020,23 +1001,23 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="D13" s="2">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1044,11 +1025,11 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="N13" s="1">
         <f t="shared" si="0"/>
-        <v>4.9384615384615387</v>
+        <v>4.6461538461538456</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1062,21 +1043,21 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="D14" s="2">
-        <v>0.13</v>
+        <v>0.18</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1084,11 +1065,11 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="N14" s="1">
         <f t="shared" si="0"/>
-        <v>5.092307692307692</v>
+        <v>4.9384615384615387</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1100,23 +1081,35 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.13</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2">
+        <v>10</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+      <c r="M15" s="2">
+        <v>300</v>
+      </c>
       <c r="N15" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.092307692307692</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1129,18 +1122,10 @@
       <c r="T15" s="1"/>
     </row>
     <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.02</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1149,12 +1134,10 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
-      <c r="M16" s="2">
-        <v>0</v>
-      </c>
+      <c r="M16" s="2"/>
       <c r="N16" s="1">
         <f t="shared" si="0"/>
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -1168,22 +1151,20 @@
     </row>
     <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
       </c>
       <c r="D17" s="2">
-        <v>0.19</v>
+        <v>0.02</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <v>17</v>
-      </c>
+      <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1194,37 +1175,35 @@
       </c>
       <c r="N17" s="1">
         <f t="shared" si="0"/>
-        <v>9.2769230769230759</v>
+        <v>-0.4</v>
       </c>
       <c r="O17" s="1"/>
-      <c r="P17" s="1">
-        <v>10.5</v>
-      </c>
+      <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1">
         <f t="shared" si="1"/>
-        <v>0.252</v>
+        <v>0</v>
       </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
     <row r="18" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C18" s="2">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -1232,39 +1211,41 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="N18" s="1">
         <f t="shared" si="0"/>
-        <v>9.5538461538461519</v>
+        <v>9.2769230769230759</v>
       </c>
       <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
+      <c r="P18" s="1">
+        <v>10.5</v>
+      </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.252</v>
       </c>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
     <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C19" s="2">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="D19" s="2">
-        <v>0.33</v>
+        <v>0.23</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1272,11 +1253,11 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="N19" s="1">
         <f t="shared" si="0"/>
-        <v>12.476923076923075</v>
+        <v>9.5538461538461519</v>
       </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1289,22 +1270,34 @@
       <c r="T19" s="1"/>
     </row>
     <row r="20" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="2">
+        <v>-4</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.33</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2">
+        <v>30</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
+      <c r="M20" s="2">
+        <v>4000</v>
+      </c>
       <c r="N20" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12.476923076923075</v>
       </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1316,35 +1309,23 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="4">
-        <v>0</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0.36</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4">
-        <v>30</v>
-      </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4">
-        <v>500</v>
-      </c>
+    <row r="21" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
       <c r="N21" s="1">
         <f t="shared" si="0"/>
-        <v>15.876923076923077</v>
+        <v>0</v>
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1356,23 +1337,35 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.36</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4">
+        <v>30</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4">
+        <v>500</v>
+      </c>
       <c r="N22" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15.876923076923077</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1385,24 +1378,22 @@
       <c r="T22" s="1"/>
     </row>
     <row r="23" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0.02</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
       <c r="N23" s="1">
         <f t="shared" si="0"/>
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -1414,28 +1405,25 @@
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>0.34</v>
-      </c>
-      <c r="G24">
-        <v>30</v>
+        <v>0.02</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
       <c r="N24" s="1">
         <f t="shared" si="0"/>
-        <v>16.276923076923076</v>
+        <v>-0.4</v>
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -1449,26 +1437,26 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C25">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>7.0000000000000007E-2</v>
+        <v>0.34</v>
       </c>
       <c r="G25">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="M25">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="N25" s="1">
         <f t="shared" si="0"/>
-        <v>15.292307692307691</v>
+        <v>16.276923076923076</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1480,28 +1468,28 @@
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C26">
-        <v>-6</v>
+        <v>9</v>
       </c>
       <c r="D26">
-        <v>0.65</v>
+        <v>0.13</v>
       </c>
       <c r="G26">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="M26">
-        <v>3000</v>
+        <v>200</v>
       </c>
       <c r="N26" s="1">
         <f t="shared" si="0"/>
-        <v>19.46153846153846</v>
+        <v>14.092307692307692</v>
       </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -1514,9 +1502,27 @@
       <c r="T26" s="1"/>
     </row>
     <row r="27" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27">
+        <v>-6</v>
+      </c>
+      <c r="D27">
+        <v>0.65</v>
+      </c>
+      <c r="G27">
+        <v>50</v>
+      </c>
+      <c r="M27">
+        <v>3000</v>
+      </c>
       <c r="N27" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19.46153846153846</v>
       </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -1529,24 +1535,9 @@
       <c r="T27" s="1"/>
     </row>
     <row r="28" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0.02</v>
-      </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
       <c r="N28" s="1">
         <f t="shared" si="0"/>
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -1559,34 +1550,24 @@
       <c r="T28" s="1"/>
     </row>
     <row r="29" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="2">
-        <v>0</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0.34</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2">
-        <v>30</v>
-      </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0.02</v>
+      </c>
+      <c r="M29">
         <v>0</v>
       </c>
       <c r="N29" s="1">
         <f t="shared" si="0"/>
-        <v>16.276923076923076</v>
+        <v>-0.4</v>
       </c>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -1600,16 +1581,16 @@
     </row>
     <row r="30" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" s="2">
-        <v>0.36</v>
+        <v>0.34</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1622,17 +1603,17 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="N30" s="1">
         <f t="shared" si="0"/>
-        <v>16.876923076923077</v>
+        <v>16.276923076923076</v>
       </c>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1">
-        <f>P30*0.024</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S30" s="1"/>
@@ -1640,21 +1621,21 @@
     </row>
     <row r="31" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C31" s="2">
-        <v>-9</v>
+        <v>1</v>
       </c>
       <c r="D31" s="2">
-        <v>0.68</v>
+        <v>0.36</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -1662,39 +1643,51 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2">
-        <v>3000</v>
+        <v>500</v>
       </c>
       <c r="N31" s="1">
         <f t="shared" si="0"/>
-        <v>15.861538461538458</v>
+        <v>16.876923076923077</v>
       </c>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1">
-        <f t="shared" si="1"/>
+        <f>P31*0.024</f>
         <v>0</v>
       </c>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
     </row>
     <row r="32" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="A32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="2">
+        <v>-9</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.68</v>
+      </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="G32" s="2">
+        <v>50</v>
+      </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
+      <c r="M32" s="2">
+        <v>3000</v>
+      </c>
       <c r="N32" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15.861538461538458</v>
       </c>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
@@ -1707,34 +1700,22 @@
       <c r="T32" s="1"/>
     </row>
     <row r="33" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0.3</v>
-      </c>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="2">
-        <v>25</v>
-      </c>
+      <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="2">
-        <v>500</v>
-      </c>
+      <c r="M33" s="2"/>
       <c r="N33" s="1">
         <f t="shared" si="0"/>
-        <v>13.23076923076923</v>
+        <v>0</v>
       </c>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
@@ -1748,21 +1729,21 @@
     </row>
     <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C34" s="2">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="D34" s="2">
-        <v>0.38</v>
+        <v>0.3</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -1770,11 +1751,11 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="N34" s="1">
         <f t="shared" si="0"/>
-        <v>13.015384615384614</v>
+        <v>13.23076923076923</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -1788,21 +1769,21 @@
     </row>
     <row r="35" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C35" s="2">
-        <v>-10</v>
+        <v>-4</v>
       </c>
       <c r="D35" s="2">
-        <v>0.46</v>
+        <v>0.38</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -1810,11 +1791,11 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="N35" s="1">
         <f t="shared" si="0"/>
-        <v>11.569230769230764</v>
+        <v>13.015384615384614</v>
       </c>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
@@ -1827,52 +1808,62 @@
       <c r="T35" s="1"/>
     </row>
     <row r="36" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+      <c r="A36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="2">
+        <v>-10</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.46</v>
+      </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="G36" s="2">
+        <v>40</v>
+      </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
+      <c r="M36" s="2">
+        <v>1000</v>
+      </c>
       <c r="N36" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11.569230769230764</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
-      <c r="R36" s="1"/>
+      <c r="R36" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
     </row>
     <row r="37" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0.35</v>
-      </c>
-      <c r="G37">
-        <v>32</v>
-      </c>
-      <c r="M37">
-        <v>500</v>
-      </c>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
       <c r="N37" s="1">
         <f t="shared" si="0"/>
-        <v>17.615384615384613</v>
+        <v>0</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
@@ -1883,29 +1874,26 @@
     </row>
     <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C38">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>0.23</v>
-      </c>
-      <c r="F38">
-        <v>-2</v>
+        <v>0.36</v>
       </c>
       <c r="G38">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="M38">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="N38" s="1">
         <f t="shared" si="0"/>
-        <v>18.984615384615381</v>
+        <v>17.415384615384614</v>
       </c>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -1916,29 +1904,29 @@
     </row>
     <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C39">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D39">
-        <v>0.12</v>
+        <v>0.23</v>
       </c>
       <c r="F39">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="G39">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M39">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="N39" s="1">
         <f t="shared" si="0"/>
-        <v>21.692307692307693</v>
+        <v>18.984615384615381</v>
       </c>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
@@ -1949,29 +1937,29 @@
     </row>
     <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C40">
-        <v>-20</v>
+        <v>14</v>
       </c>
       <c r="D40">
-        <v>0.6</v>
+        <v>0.12</v>
+      </c>
+      <c r="F40">
+        <v>-4</v>
       </c>
       <c r="G40">
-        <v>50</v>
-      </c>
-      <c r="H40">
-        <v>0.05</v>
+        <v>10</v>
       </c>
       <c r="M40">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="N40" s="1">
         <f t="shared" si="0"/>
-        <v>6.2115384615384599</v>
+        <v>21.692307692307693</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -1982,26 +1970,29 @@
     </row>
     <row r="41" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C41">
-        <v>-5</v>
+        <v>-20</v>
       </c>
       <c r="D41">
-        <v>0.11</v>
+        <v>0.6</v>
       </c>
       <c r="G41">
-        <v>10</v>
+        <v>50</v>
+      </c>
+      <c r="H41">
+        <v>0.05</v>
       </c>
       <c r="M41">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="N41" s="1">
         <f t="shared" si="0"/>
-        <v>0.49230769230769145</v>
+        <v>6.2115384615384599</v>
       </c>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
@@ -2012,35 +2003,26 @@
     </row>
     <row r="42" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C42">
-        <v>-45</v>
+        <v>-5</v>
       </c>
       <c r="D42">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E42">
-        <v>20</v>
-      </c>
-      <c r="F42">
-        <v>20</v>
+        <v>0.11</v>
       </c>
       <c r="G42">
-        <v>50</v>
-      </c>
-      <c r="H42">
-        <v>0.05</v>
+        <v>10</v>
       </c>
       <c r="M42">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="N42" s="1">
         <f t="shared" si="0"/>
-        <v>-45.78846153846154</v>
+        <v>0.49230769230769145</v>
       </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
@@ -2051,23 +2033,35 @@
     </row>
     <row r="43" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C43">
-        <v>-2</v>
+        <v>-45</v>
       </c>
       <c r="D43">
-        <v>0.1</v>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E43">
+        <v>20</v>
+      </c>
+      <c r="F43">
+        <v>20</v>
+      </c>
+      <c r="G43">
+        <v>50</v>
+      </c>
+      <c r="H43">
+        <v>0.05</v>
       </c>
       <c r="M43">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="N43" s="1">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-46.188461538461546</v>
       </c>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
@@ -2077,9 +2071,24 @@
       <c r="T43" s="1"/>
     </row>
     <row r="44" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44">
+        <v>-2</v>
+      </c>
+      <c r="D44">
+        <v>0.1</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
       <c r="N44" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
@@ -2436,7 +2445,18 @@
       <c r="S73" s="1"/>
       <c r="T73" s="1"/>
     </row>
-    <row r="74" spans="14:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="14:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N74" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+    </row>
     <row r="75" spans="14:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="14:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="77" spans="14:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3360,6 +3380,7 @@
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>